<commit_message>
pytest codes, RAG flow diagram
</commit_message>
<xml_diff>
--- a/data/qa_with_predictions_part2.xlsx
+++ b/data/qa_with_predictions_part2.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D985"/>
+  <dimension ref="A1:D1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24917,6 +24917,312 @@
         </is>
       </c>
     </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>When did trench warfare become archetypically associated with?</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>World War I (1914-1918)</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>World War I.</t>
+        </is>
+      </c>
+      <c r="D986" t="inlineStr"/>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>What type of land warfare is characterized by occupied lines comprising military trenches?</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Trench warfare</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>Trench warfare.</t>
+        </is>
+      </c>
+      <c r="D987" t="inlineStr"/>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>What was the result of a revolution in firepower not being matched by advances in mobility?</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Trench warfare proliferated.</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>The Napoleonic Wars.</t>
+        </is>
+      </c>
+      <c r="D988" t="inlineStr"/>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>What area between opposing trench lines was fully exposed to artillery fire from both sides?</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>No man's land.</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>No Man's Land.</t>
+        </is>
+      </c>
+      <c r="D989" t="inlineStr"/>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>When did Roman legions entrench camps nightly when on the move?</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>In the presence of an enemy.</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>Roman legions entrenched their camps nightly when on the move during the 2nd century BC to around the 2nd century AD.</t>
+        </is>
+      </c>
+      <c r="D990" t="inlineStr"/>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>Who suggested digging a trench to defend Medina in 627 AD?</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Salman the Persian</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>Khalid ibn al-Walid.</t>
+        </is>
+      </c>
+      <c r="D991" t="inlineStr"/>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>What was the date when French soldiers captured the left bank of the Po river?</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>May 12, 1640.</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>March 26, 1797.</t>
+        </is>
+      </c>
+      <c r="D992" t="inlineStr"/>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>How many times did the French soldiers' advance on trenches get repelled?</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Twice.</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>Three.</t>
+        </is>
+      </c>
+      <c r="D993" t="inlineStr"/>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>Where did the defenders flee to seek sanctuary?</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>The Santa Maria al Monte dei Cappuccini church in Turin.</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>Rome.</t>
+        </is>
+      </c>
+      <c r="D994" t="inlineStr"/>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>How many times did the French break through before succeeding?</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>On the third attempt.</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>The French broke through three times before succeeding at the Battle of Austerlitz on December 2, 1805.</t>
+        </is>
+      </c>
+      <c r="D995" t="inlineStr"/>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>What was the purpose of field works in early modern warfare?</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>To block possible lines of advance.</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>To gather intelligence and identify enemy positions, fortifications, and troop movements.</t>
+        </is>
+      </c>
+      <c r="D996" t="inlineStr"/>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>In which year were the Lines of Torres Vedras built?</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>1809 and 1810.</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>1809.</t>
+        </is>
+      </c>
+      <c r="D997" t="inlineStr"/>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>When did the Māori develop elaborate trench and bunker systems?</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>1845-1872</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>The Māori did not develop elaborate trench and bunker systems.</t>
+        </is>
+      </c>
+      <c r="D998" t="inlineStr"/>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>What was often considered to be the most sophisticated pā by historians?</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Ruapekapeka</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>The Taupo Pā.</t>
+        </is>
+      </c>
+      <c r="D999" t="inlineStr"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>When did James Belich write his book on the New Zealand Wars?</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>1980s</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>1865.</t>
+        </is>
+      </c>
+      <c r="D1000" t="inlineStr"/>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>What is the name of the historian who criticized James Belich's claim about Māori inventing trench warfare?</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Gavin McLean</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>Keith Sinclair.</t>
+        </is>
+      </c>
+      <c r="D1001" t="inlineStr"/>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>Who did the Māori not invent trench warfare first?</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Not specified (but implied to be someone else)</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>The British.</t>
+        </is>
+      </c>
+      <c r="D1002" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>